<commit_message>
flattening logic update for json node and corresponding changes
</commit_message>
<xml_diff>
--- a/src/main/resources/master_json_arrayTest.xlsx
+++ b/src/main/resources/master_json_arrayTest.xlsx
@@ -14,22 +14,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="304">
   <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
     <t>userId</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>body</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>sunt aut facere repellat provident occaecati excepturi optio reprehenderit</t>
   </si>
   <si>
     <t>quia et suscipit
@@ -38,10 +32,10 @@
 nostrum rerum est autem sunt rem eveniet architecto</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>qui est esse</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>sunt aut facere repellat provident occaecati excepturi optio reprehenderit</t>
   </si>
   <si>
     <t>est rerum tempore vitae
@@ -50,10 +44,10 @@
 qui aperiam non debitis possimus qui neque nisi nulla</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>ea molestias quasi exercitationem repellat qui ipsa sit aut</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>qui est esse</t>
   </si>
   <si>
     <t>et iusto sed quo iure
@@ -62,10 +56,10 @@
 molestiae porro eius odio et labore et velit aut</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>eum et est occaecati</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>ea molestias quasi exercitationem repellat qui ipsa sit aut</t>
   </si>
   <si>
     <t>ullam et saepe reiciendis voluptatem adipisci
@@ -74,10 +68,10 @@
 quis sunt voluptatem rerum illo velit</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>nesciunt quas odio</t>
+    <t>4</t>
+  </si>
+  <si>
+    <t>eum et est occaecati</t>
   </si>
   <si>
     <t>repudiandae veniam quaerat sunt sed
@@ -86,10 +80,10 @@
 est aut tenetur dolor neque</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>dolorem eum magni eos aperiam quia</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>nesciunt quas odio</t>
   </si>
   <si>
     <t>ut aspernatur corporis harum nihil quis provident sequi
@@ -98,10 +92,10 @@
 voluptate dolores velit et doloremque molestiae</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>magnam facilis autem</t>
+    <t>6</t>
+  </si>
+  <si>
+    <t>dolorem eum magni eos aperiam quia</t>
   </si>
   <si>
     <t>dolore placeat quibusdam ea quo vitae
@@ -110,10 +104,10 @@
 sunt ut sequi eos ea sed quas</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>dolorem dolore est ipsam</t>
+    <t>7</t>
+  </si>
+  <si>
+    <t>magnam facilis autem</t>
   </si>
   <si>
     <t>dignissimos aperiam dolorem qui eum
@@ -122,10 +116,10 @@
 ipsam ut commodi dolor voluptatum modi aut vitae</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>nesciunt iure omnis dolorem tempora et accusantium</t>
+    <t>8</t>
+  </si>
+  <si>
+    <t>dolorem dolore est ipsam</t>
   </si>
   <si>
     <t>consectetur animi nesciunt iure dolore
@@ -134,10 +128,10 @@
 et est aut quod aut provident voluptas autem voluptas</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>optio molestias id quia eum</t>
+    <t>9</t>
+  </si>
+  <si>
+    <t>nesciunt iure omnis dolorem tempora et accusantium</t>
   </si>
   <si>
     <t>quo et expedita modi cum officia vel magni
@@ -146,10 +140,10 @@
 quos veniam quod sed accusamus veritatis error</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>et ea vero quia laudantium autem</t>
+    <t>10</t>
+  </si>
+  <si>
+    <t>optio molestias id quia eum</t>
   </si>
   <si>
     <t>delectus reiciendis molestiae occaecati non minima eveniet qui voluptatibus
@@ -158,10 +152,10 @@
 ut animi commodi</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>in quibusdam tempore odit est dolorem</t>
+    <t>11</t>
+  </si>
+  <si>
+    <t>et ea vero quia laudantium autem</t>
   </si>
   <si>
     <t>itaque id aut magnam
@@ -170,10 +164,10 @@
 incidunt ea est distinctio odio</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>dolorum ut in voluptas mollitia et saepe quo animi</t>
+    <t>12</t>
+  </si>
+  <si>
+    <t>in quibusdam tempore odit est dolorem</t>
   </si>
   <si>
     <t>aut dicta possimus sint mollitia voluptas commodi quo doloremque
@@ -182,10 +176,10 @@
 perferendis recusandae assumenda consectetur porro architecto ipsum ipsam</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>voluptatem eligendi optio</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>dolorum ut in voluptas mollitia et saepe quo animi</t>
   </si>
   <si>
     <t>fuga et accusamus dolorum perferendis illo voluptas
@@ -194,10 +188,10 @@
 sed aut voluptas totam sit illum</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>eveniet quod temporibus</t>
+    <t>14</t>
+  </si>
+  <si>
+    <t>voluptatem eligendi optio</t>
   </si>
   <si>
     <t>reprehenderit quos placeat
@@ -206,10 +200,10 @@
 officiis harum fugiat vitae</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>sint suscipit perspiciatis velit dolorum rerum ipsa laboriosam odio</t>
+    <t>15</t>
+  </si>
+  <si>
+    <t>eveniet quod temporibus</t>
   </si>
   <si>
     <t>suscipit nam nisi quo aperiam aut
@@ -218,10 +212,10 @@
 consequatur magni mollitia accusamus ea nisi voluptate dicta</t>
   </si>
   <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>fugit voluptas sed molestias voluptatem provident</t>
+    <t>16</t>
+  </si>
+  <si>
+    <t>sint suscipit perspiciatis velit dolorum rerum ipsa laboriosam odio</t>
   </si>
   <si>
     <t>eos voluptas et aut odit natus earum
@@ -230,10 +224,10 @@
 qui nihil ratione nemo velit ut aut id quo</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>voluptate et itaque vero tempora molestiae</t>
+    <t>17</t>
+  </si>
+  <si>
+    <t>fugit voluptas sed molestias voluptatem provident</t>
   </si>
   <si>
     <t>eveniet quo quis
@@ -242,10 +236,10 @@
 est voluptatem vel debitis et magnam</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>adipisci placeat illum aut reiciendis qui</t>
+    <t>18</t>
+  </si>
+  <si>
+    <t>voluptate et itaque vero tempora molestiae</t>
   </si>
   <si>
     <t>illum quis cupiditate provident sit magnam
@@ -254,10 +248,10 @@
 adipisci quo iste expedita sit quos voluptas</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>doloribus ad provident suscipit at</t>
+    <t>19</t>
+  </si>
+  <si>
+    <t>adipisci placeat illum aut reiciendis qui</t>
   </si>
   <si>
     <t>qui consequuntur ducimus possimus quisquam amet similique
@@ -266,10 +260,10 @@
 omnis rerum consequatur expedita quidem cumque explicabo</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>asperiores ea ipsam voluptatibus modi minima quia sint</t>
+    <t>20</t>
+  </si>
+  <si>
+    <t>doloribus ad provident suscipit at</t>
   </si>
   <si>
     <t>repellat aliquid praesentium dolorem quo
@@ -278,10 +272,10 @@
 tempora et tenetur expedita sunt</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>dolor sint quo a velit explicabo quia nam</t>
+    <t>21</t>
+  </si>
+  <si>
+    <t>asperiores ea ipsam voluptatibus modi minima quia sint</t>
   </si>
   <si>
     <t>eos qui et ipsum ipsam suscipit aut
@@ -290,10 +284,10 @@
 nam impedit esse</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>maxime id vitae nihil numquam</t>
+    <t>22</t>
+  </si>
+  <si>
+    <t>dolor sint quo a velit explicabo quia nam</t>
   </si>
   <si>
     <t>veritatis unde neque eligendi
@@ -302,10 +296,10 @@
 et et vel beatae sequi ullam sed tenetur perspiciatis</t>
   </si>
   <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>autem hic labore sunt dolores incidunt</t>
+    <t>23</t>
+  </si>
+  <si>
+    <t>maxime id vitae nihil numquam</t>
   </si>
   <si>
     <t>enim et ex nulla
@@ -314,10 +308,10 @@
 totam recusandae id dignissimos aut sed asperiores deserunt</t>
   </si>
   <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>rem alias distinctio quo quis</t>
+    <t>24</t>
+  </si>
+  <si>
+    <t>autem hic labore sunt dolores incidunt</t>
   </si>
   <si>
     <t>ullam consequatur ut
@@ -326,10 +320,10 @@
 molestiae illo tempore quia et distinctio</t>
   </si>
   <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>est et quae odit qui non</t>
+    <t>25</t>
+  </si>
+  <si>
+    <t>rem alias distinctio quo quis</t>
   </si>
   <si>
     <t>similique esse doloribus nihil accusamus
@@ -338,10 +332,10 @@
 omnis aut molestiae vel vero</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>quasi id et eos tenetur aut quo autem</t>
+    <t>26</t>
+  </si>
+  <si>
+    <t>est et quae odit qui non</t>
   </si>
   <si>
     <t>eum sed dolores ipsam sint possimus debitis occaecati
@@ -350,10 +344,10 @@
 consequatur suscipit necessitatibus rerum sed inventore temporibus consequatur</t>
   </si>
   <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>delectus ullam et corporis nulla voluptas sequi</t>
+    <t>27</t>
+  </si>
+  <si>
+    <t>quasi id et eos tenetur aut quo autem</t>
   </si>
   <si>
     <t>non et quaerat ex quae ad maiores
@@ -362,10 +356,10 @@
 similique nostrum eum</t>
   </si>
   <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>iusto eius quod necessitatibus culpa ea</t>
+    <t>28</t>
+  </si>
+  <si>
+    <t>delectus ullam et corporis nulla voluptas sequi</t>
   </si>
   <si>
     <t>odit magnam ut saepe sed non qui
@@ -374,10 +368,10 @@
 eligendi repudiandae odit magni similique sed cum maiores</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>a quo magni similique perferendis</t>
+    <t>29</t>
+  </si>
+  <si>
+    <t>iusto eius quod necessitatibus culpa ea</t>
   </si>
   <si>
     <t>alias dolor cumque
@@ -386,10 +380,10 @@
 a provident perspiciatis quia</t>
   </si>
   <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>ullam ut quidem id aut vel consequuntur</t>
+    <t>30</t>
+  </si>
+  <si>
+    <t>a quo magni similique perferendis</t>
   </si>
   <si>
     <t>debitis eius sed quibusdam non quis consectetur vitae
@@ -398,10 +392,10 @@
 quaerat voluptatem adipisci repudiandae</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>doloremque illum aliquid sunt</t>
+    <t>31</t>
+  </si>
+  <si>
+    <t>ullam ut quidem id aut vel consequuntur</t>
   </si>
   <si>
     <t>deserunt eos nobis asperiores et hic
@@ -410,10 +404,10 @@
 earum voluptates et aut adipisci ea maiores voluptas maxime</t>
   </si>
   <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>qui explicabo molestiae dolorem</t>
+    <t>32</t>
+  </si>
+  <si>
+    <t>doloremque illum aliquid sunt</t>
   </si>
   <si>
     <t>rerum ut et numquam laborum odit est sit
@@ -422,10 +416,10 @@
 rerum officiis sequi cumque quod</t>
   </si>
   <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>magnam ut rerum iure</t>
+    <t>33</t>
+  </si>
+  <si>
+    <t>qui explicabo molestiae dolorem</t>
   </si>
   <si>
     <t>ea velit perferendis earum ut voluptatem voluptate itaque iusto
@@ -434,10 +428,10 @@
 est distinctio qui assumenda accusamus dignissimos officia nesciunt nobis</t>
   </si>
   <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>id nihil consequatur molestias animi provident</t>
+    <t>34</t>
+  </si>
+  <si>
+    <t>magnam ut rerum iure</t>
   </si>
   <si>
     <t>nisi error delectus possimus ut eligendi vitae
@@ -446,10 +440,10 @@
 et nobis quia fugit</t>
   </si>
   <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>fuga nam accusamus voluptas reiciendis itaque</t>
+    <t>35</t>
+  </si>
+  <si>
+    <t>id nihil consequatur molestias animi provident</t>
   </si>
   <si>
     <t>ad mollitia et omnis minus architecto odit
@@ -458,10 +452,10 @@
 qui aspernatur quia eaque ut aperiam inventore</t>
   </si>
   <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>provident vel ut sit ratione est</t>
+    <t>36</t>
+  </si>
+  <si>
+    <t>fuga nam accusamus voluptas reiciendis itaque</t>
   </si>
   <si>
     <t>debitis et eaque non officia sed nesciunt pariatur vel
@@ -470,10 +464,10 @@
 voluptates omnis consequatur aut enim officiis in quam qui</t>
   </si>
   <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>explicabo et eos deleniti nostrum ab id repellendus</t>
+    <t>37</t>
+  </si>
+  <si>
+    <t>provident vel ut sit ratione est</t>
   </si>
   <si>
     <t>animi esse sit aut sit nesciunt assumenda eum voluptas
@@ -482,10 +476,10 @@
 ratione optio eos iusto veniam iure</t>
   </si>
   <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>eos dolorem iste accusantium est eaque quam</t>
+    <t>38</t>
+  </si>
+  <si>
+    <t>explicabo et eos deleniti nostrum ab id repellendus</t>
   </si>
   <si>
     <t>corporis rerum ducimus vel eum accusantium
@@ -494,10 +488,10 @@
 voluptas sapiente vel dolore minus voluptatem incidunt ex</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>enim quo cumque</t>
+    <t>39</t>
+  </si>
+  <si>
+    <t>eos dolorem iste accusantium est eaque quam</t>
   </si>
   <si>
     <t>ut voluptatum aliquid illo tenetur nemo sequi quo facilis
@@ -506,10 +500,10 @@
 unde omnis voluptatem iure quasi maxime voluptas nam</t>
   </si>
   <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>non est facere</t>
+    <t>40</t>
+  </si>
+  <si>
+    <t>enim quo cumque</t>
   </si>
   <si>
     <t>molestias id nostrum
@@ -518,10 +512,10 @@
 nam quidem est ducimus sunt debitis saepe</t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>commodi ullam sint et excepturi error explicabo praesentium voluptas</t>
+    <t>41</t>
+  </si>
+  <si>
+    <t>non est facere</t>
   </si>
   <si>
     <t>odio fugit voluptatum ducimus earum autem est incidunt voluptatem
@@ -530,10 +524,10 @@
 ratione harum vitae ut</t>
   </si>
   <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>eligendi iste nostrum consequuntur adipisci praesentium sit beatae perferendis</t>
+    <t>42</t>
+  </si>
+  <si>
+    <t>commodi ullam sint et excepturi error explicabo praesentium voluptas</t>
   </si>
   <si>
     <t>similique fugit est
@@ -542,10 +536,10 @@
 dolorum exercitationem magnam ex et a et distinctio debitis</t>
   </si>
   <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>optio dolor molestias sit</t>
+    <t>43</t>
+  </si>
+  <si>
+    <t>eligendi iste nostrum consequuntur adipisci praesentium sit beatae perferendis</t>
   </si>
   <si>
     <t>temporibus est consectetur dolore
@@ -554,10 +548,10 @@
 ea et iure quam sed maxime ut distinctio quae</t>
   </si>
   <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>ut numquam possimus omnis eius suscipit laudantium iure</t>
+    <t>44</t>
+  </si>
+  <si>
+    <t>optio dolor molestias sit</t>
   </si>
   <si>
     <t>est natus reiciendis nihil possimus aut provident
@@ -566,10 +560,10 @@
 nobis rerum repellendus dolorem autem</t>
   </si>
   <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>aut quo modi neque nostrum ducimus</t>
+    <t>45</t>
+  </si>
+  <si>
+    <t>ut numquam possimus omnis eius suscipit laudantium iure</t>
   </si>
   <si>
     <t>voluptatem quisquam iste
@@ -578,10 +572,10 @@
 vel et voluptatum in aliquid</t>
   </si>
   <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>quibusdam cumque rem aut deserunt</t>
+    <t>46</t>
+  </si>
+  <si>
+    <t>aut quo modi neque nostrum ducimus</t>
   </si>
   <si>
     <t>voluptatem assumenda ut qui ut cupiditate aut impedit veniam
@@ -590,10 +584,10 @@
 eligendi et voluptate</t>
   </si>
   <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>ut voluptatem illum ea doloribus itaque eos</t>
+    <t>47</t>
+  </si>
+  <si>
+    <t>quibusdam cumque rem aut deserunt</t>
   </si>
   <si>
     <t>voluptates quo voluptatem facilis iure occaecati
@@ -602,10 +596,10 @@
 laudantium repellat ad ut et autem reprehenderit</t>
   </si>
   <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>laborum non sunt aut ut assumenda perspiciatis voluptas</t>
+    <t>48</t>
+  </si>
+  <si>
+    <t>ut voluptatem illum ea doloribus itaque eos</t>
   </si>
   <si>
     <t>inventore ab sint
@@ -614,10 +608,10 @@
 quibusdam officiis aspernatur cumque aut commodi aut</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>repellendus qui recusandae incidunt voluptates tenetur qui omnis exercitationem</t>
+    <t>49</t>
+  </si>
+  <si>
+    <t>laborum non sunt aut ut assumenda perspiciatis voluptas</t>
   </si>
   <si>
     <t>error suscipit maxime adipisci consequuntur recusandae
@@ -626,10 +620,10 @@
 adipisci impedit sequi nesciunt quis consectetur</t>
   </si>
   <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>soluta aliquam aperiam consequatur illo quis voluptas</t>
+    <t>50</t>
+  </si>
+  <si>
+    <t>repellendus qui recusandae incidunt voluptates tenetur qui omnis exercitationem</t>
   </si>
   <si>
     <t>sunt dolores aut doloribus
@@ -638,10 +632,10 @@
 cum asperiores sit consectetur dolorem</t>
   </si>
   <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>qui enim et consequuntur quia animi quis voluptate quibusdam</t>
+    <t>51</t>
+  </si>
+  <si>
+    <t>soluta aliquam aperiam consequatur illo quis voluptas</t>
   </si>
   <si>
     <t>iusto est quibusdam fuga quas quaerat molestias
@@ -650,10 +644,10 @@
 soluta esse reprehenderit qui laborum</t>
   </si>
   <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>ut quo aut ducimus alias</t>
+    <t>52</t>
+  </si>
+  <si>
+    <t>qui enim et consequuntur quia animi quis voluptate quibusdam</t>
   </si>
   <si>
     <t>minima harum praesentium eum rerum illo dolore
@@ -662,10 +656,10 @@
 consequatur minus dolor quidem veritatis sunt non explicabo similique</t>
   </si>
   <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>sit asperiores ipsam eveniet odio non quia</t>
+    <t>53</t>
+  </si>
+  <si>
+    <t>ut quo aut ducimus alias</t>
   </si>
   <si>
     <t>totam corporis dignissimos
@@ -674,10 +668,10 @@
 et exercitationem vero incidunt corrupti mollitia</t>
   </si>
   <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>sit vel voluptatem et non libero</t>
+    <t>54</t>
+  </si>
+  <si>
+    <t>sit asperiores ipsam eveniet odio non quia</t>
   </si>
   <si>
     <t>debitis excepturi ea perferendis harum libero optio
@@ -686,10 +680,10 @@
 nihil ut eum odit</t>
   </si>
   <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>qui et at rerum necessitatibus</t>
+    <t>55</t>
+  </si>
+  <si>
+    <t>sit vel voluptatem et non libero</t>
   </si>
   <si>
     <t>aut est omnis dolores
@@ -698,10 +692,10 @@
 corporis harum reprehenderit dolores eligendi</t>
   </si>
   <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t>sed ab est est</t>
+    <t>56</t>
+  </si>
+  <si>
+    <t>qui et at rerum necessitatibus</t>
   </si>
   <si>
     <t>at pariatur consequuntur earum quidem
@@ -710,10 +704,10 @@
 et cum voluptas voluptatum repellat est</t>
   </si>
   <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t>voluptatum itaque dolores nisi et quasi</t>
+    <t>57</t>
+  </si>
+  <si>
+    <t>sed ab est est</t>
   </si>
   <si>
     <t>veniam voluptatum quae adipisci id
@@ -722,10 +716,10 @@
 ad similique veniam</t>
   </si>
   <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>qui commodi dolor at maiores et quis id accusantium</t>
+    <t>58</t>
+  </si>
+  <si>
+    <t>voluptatum itaque dolores nisi et quasi</t>
   </si>
   <si>
     <t>perspiciatis et quam ea autem temporibus non voluptatibus qui
@@ -734,10 +728,10 @@
 et hic ut ut commodi expedita sunt</t>
   </si>
   <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>consequatur placeat omnis quisquam quia reprehenderit fugit veritatis facere</t>
+    <t>59</t>
+  </si>
+  <si>
+    <t>qui commodi dolor at maiores et quis id accusantium</t>
   </si>
   <si>
     <t>asperiores sunt ab assumenda cumque modi velit
@@ -746,10 +740,10 @@
 illo ratione amet aut et omnis</t>
   </si>
   <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>voluptatem doloribus consectetur est ut ducimus</t>
+    <t>60</t>
+  </si>
+  <si>
+    <t>consequatur placeat omnis quisquam quia reprehenderit fugit veritatis facere</t>
   </si>
   <si>
     <t>ab nemo optio odio
@@ -758,10 +752,10 @@
 magnam minus velit</t>
   </si>
   <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>beatae enim quia vel</t>
+    <t>61</t>
+  </si>
+  <si>
+    <t>voluptatem doloribus consectetur est ut ducimus</t>
   </si>
   <si>
     <t>enim aspernatur illo distinctio quae praesentium
@@ -770,10 +764,10 @@
 quo molestiae omnis ea eveniet optio</t>
   </si>
   <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>voluptas blanditiis repellendus animi ducimus error sapiente et suscipit</t>
+    <t>62</t>
+  </si>
+  <si>
+    <t>beatae enim quia vel</t>
   </si>
   <si>
     <t>enim adipisci aspernatur nemo
@@ -782,10 +776,10 @@
 accusantium ut quam in voluptatibus voluptas ipsam dicta</t>
   </si>
   <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>et fugit quas eum in in aperiam quod</t>
+    <t>63</t>
+  </si>
+  <si>
+    <t>voluptas blanditiis repellendus animi ducimus error sapiente et suscipit</t>
   </si>
   <si>
     <t>id velit blanditiis
@@ -794,10 +788,10 @@
 incidunt a error provident eaque aut aut qui</t>
   </si>
   <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>consequatur id enim sunt et et</t>
+    <t>64</t>
+  </si>
+  <si>
+    <t>et fugit quas eum in in aperiam quod</t>
   </si>
   <si>
     <t>voluptatibus ex esse
@@ -806,10 +800,10 @@
 natus id esse incidunt pariatur</t>
   </si>
   <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>repudiandae ea animi iusto</t>
+    <t>65</t>
+  </si>
+  <si>
+    <t>consequatur id enim sunt et et</t>
   </si>
   <si>
     <t>officia veritatis tenetur vero qui itaque
@@ -818,10 +812,10 @@
 veritatis quibusdam et nemo iusto saepe</t>
   </si>
   <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>aliquid eos sed fuga est maxime repellendus</t>
+    <t>66</t>
+  </si>
+  <si>
+    <t>repudiandae ea animi iusto</t>
   </si>
   <si>
     <t>reprehenderit id nostrum
@@ -830,10 +824,10 @@
 non sapiente et consequatur necessitatibus molestiae</t>
   </si>
   <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>odio quis facere architecto reiciendis optio</t>
+    <t>67</t>
+  </si>
+  <si>
+    <t>aliquid eos sed fuga est maxime repellendus</t>
   </si>
   <si>
     <t>magnam molestiae perferendis quisquam
@@ -842,10 +836,10 @@
 ea quia deleniti quidem saepe porro velit</t>
   </si>
   <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>fugiat quod pariatur odit minima</t>
+    <t>68</t>
+  </si>
+  <si>
+    <t>odio quis facere architecto reiciendis optio</t>
   </si>
   <si>
     <t>officiis error culpa consequatur modi asperiores et
@@ -854,10 +848,10 @@
 sequi commodi repudiandae asperiores et saepe a</t>
   </si>
   <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>voluptatem laborum magni</t>
+    <t>69</t>
+  </si>
+  <si>
+    <t>fugiat quod pariatur odit minima</t>
   </si>
   <si>
     <t>sunt repellendus quae
@@ -866,10 +860,10 @@
 eum tempora esse dolore</t>
   </si>
   <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>et iusto veniam et illum aut fuga</t>
+    <t>70</t>
+  </si>
+  <si>
+    <t>voluptatem laborum magni</t>
   </si>
   <si>
     <t>occaecati a doloribus
@@ -878,10 +872,10 @@
 rerum ut id enim velit est perferendis</t>
   </si>
   <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>sint hic doloribus consequatur eos non id</t>
+    <t>71</t>
+  </si>
+  <si>
+    <t>et iusto veniam et illum aut fuga</t>
   </si>
   <si>
     <t>quam occaecati qui deleniti consectetur
@@ -890,10 +884,10 @@
 sunt consectetur expedita inventore velit</t>
   </si>
   <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>consequuntur deleniti eos quia temporibus ab aliquid at</t>
+    <t>72</t>
+  </si>
+  <si>
+    <t>sint hic doloribus consequatur eos non id</t>
   </si>
   <si>
     <t>voluptatem cumque tenetur consequatur expedita ipsum nemo quia explicabo
@@ -902,10 +896,10 @@
 et in consequuntur voluptatem voluptates aut</t>
   </si>
   <si>
-    <t>74</t>
-  </si>
-  <si>
-    <t>enim unde ratione doloribus quas enim ut sit sapiente</t>
+    <t>73</t>
+  </si>
+  <si>
+    <t>consequuntur deleniti eos quia temporibus ab aliquid at</t>
   </si>
   <si>
     <t>odit qui et et necessitatibus sint veniam
@@ -914,10 +908,10 @@
 quo et tenetur ratione occaecati molestiae tempora</t>
   </si>
   <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>dignissimos eum dolor ut enim et delectus in</t>
+    <t>74</t>
+  </si>
+  <si>
+    <t>enim unde ratione doloribus quas enim ut sit sapiente</t>
   </si>
   <si>
     <t>commodi non non omnis et voluptas sit
@@ -926,10 +920,10 @@
 rerum amet et nemo voluptate expedita adipisci error dolorem</t>
   </si>
   <si>
-    <t>76</t>
-  </si>
-  <si>
-    <t>doloremque officiis ad et non perferendis</t>
+    <t>75</t>
+  </si>
+  <si>
+    <t>dignissimos eum dolor ut enim et delectus in</t>
   </si>
   <si>
     <t>ut animi facere
@@ -938,10 +932,10 @@
 quaerat recusandae totam odio</t>
   </si>
   <si>
-    <t>77</t>
-  </si>
-  <si>
-    <t>necessitatibus quasi exercitationem odio</t>
+    <t>76</t>
+  </si>
+  <si>
+    <t>doloremque officiis ad et non perferendis</t>
   </si>
   <si>
     <t>modi ut in nulla repudiandae dolorum nostrum eos
@@ -950,10 +944,10 @@
 voluptates sapiente aliquam asperiores nobis amet corrupti repudiandae provident</t>
   </si>
   <si>
-    <t>78</t>
-  </si>
-  <si>
-    <t>quam voluptatibus rerum veritatis</t>
+    <t>77</t>
+  </si>
+  <si>
+    <t>necessitatibus quasi exercitationem odio</t>
   </si>
   <si>
     <t>nobis facilis odit tempore cupiditate quia
@@ -962,10 +956,10 @@
 aut veniam repellendus</t>
   </si>
   <si>
-    <t>79</t>
-  </si>
-  <si>
-    <t>pariatur consequatur quia magnam autem omnis non amet</t>
+    <t>78</t>
+  </si>
+  <si>
+    <t>quam voluptatibus rerum veritatis</t>
   </si>
   <si>
     <t>libero accusantium et et facere incidunt sit dolorem
@@ -974,10 +968,10 @@
 officiis esse molestiae iste et quos</t>
   </si>
   <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>labore in ex et explicabo corporis aut quas</t>
+    <t>79</t>
+  </si>
+  <si>
+    <t>pariatur consequatur quia magnam autem omnis non amet</t>
   </si>
   <si>
     <t>ex quod dolorem ea eum iure qui provident amet
@@ -986,10 +980,10 @@
 minus incidunt vero fugit rerum sint sunt excepturi provident</t>
   </si>
   <si>
-    <t>81</t>
-  </si>
-  <si>
-    <t>tempora rem veritatis voluptas quo dolores vero</t>
+    <t>80</t>
+  </si>
+  <si>
+    <t>labore in ex et explicabo corporis aut quas</t>
   </si>
   <si>
     <t>facere qui nesciunt est voluptatum voluptatem nisi
@@ -998,10 +992,10 @@
 ex officiis minima doloremque voluptas ut aut</t>
   </si>
   <si>
-    <t>82</t>
-  </si>
-  <si>
-    <t>laudantium voluptate suscipit sunt enim enim</t>
+    <t>81</t>
+  </si>
+  <si>
+    <t>tempora rem veritatis voluptas quo dolores vero</t>
   </si>
   <si>
     <t>ut libero sit aut totam inventore sunt
@@ -1010,10 +1004,10 @@
 dolor enim assumenda soluta laboriosam amet iste delectus hic</t>
   </si>
   <si>
-    <t>83</t>
-  </si>
-  <si>
-    <t>odit et voluptates doloribus alias odio et</t>
+    <t>82</t>
+  </si>
+  <si>
+    <t>laudantium voluptate suscipit sunt enim enim</t>
   </si>
   <si>
     <t>est molestiae facilis quis tempora numquam nihil qui
@@ -1022,10 +1016,10 @@
 reprehenderit eius rem quibusdam</t>
   </si>
   <si>
-    <t>84</t>
-  </si>
-  <si>
-    <t>optio ipsam molestias necessitatibus occaecati facilis veritatis dolores aut</t>
+    <t>83</t>
+  </si>
+  <si>
+    <t>odit et voluptates doloribus alias odio et</t>
   </si>
   <si>
     <t>sint molestiae magni a et quos
@@ -1034,10 +1028,10 @@
 recusandae dignissimos dolor incidunt consequatur odio</t>
   </si>
   <si>
-    <t>85</t>
-  </si>
-  <si>
-    <t>dolore veritatis porro provident adipisci blanditiis et sunt</t>
+    <t>84</t>
+  </si>
+  <si>
+    <t>optio ipsam molestias necessitatibus occaecati facilis veritatis dolores aut</t>
   </si>
   <si>
     <t>similique sed nisi voluptas iusto omnis
@@ -1046,10 +1040,10 @@
 enim provident pariatur praesentium atque animi amet ratione</t>
   </si>
   <si>
-    <t>86</t>
-  </si>
-  <si>
-    <t>placeat quia et porro iste</t>
+    <t>85</t>
+  </si>
+  <si>
+    <t>dolore veritatis porro provident adipisci blanditiis et sunt</t>
   </si>
   <si>
     <t>quasi excepturi consequatur iste autem temporibus sed molestiae beatae
@@ -1058,10 +1052,10 @@
 asperiores pariatur deserunt optio</t>
   </si>
   <si>
-    <t>87</t>
-  </si>
-  <si>
-    <t>nostrum quis quasi placeat</t>
+    <t>86</t>
+  </si>
+  <si>
+    <t>placeat quia et porro iste</t>
   </si>
   <si>
     <t>eos et molestiae
@@ -1070,10 +1064,10 @@
 magnam sint rem ipsum est</t>
   </si>
   <si>
-    <t>88</t>
-  </si>
-  <si>
-    <t>sapiente omnis fugit eos</t>
+    <t>87</t>
+  </si>
+  <si>
+    <t>nostrum quis quasi placeat</t>
   </si>
   <si>
     <t>consequatur omnis est praesentium
@@ -1082,10 +1076,10 @@
 voluptatibus veniam cum et rerum sed</t>
   </si>
   <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>sint soluta et vel magnam aut ut sed qui</t>
+    <t>88</t>
+  </si>
+  <si>
+    <t>sapiente omnis fugit eos</t>
   </si>
   <si>
     <t>repellat aut aperiam totam temporibus autem et
@@ -1094,10 +1088,10 @@
 tempore quas est</t>
   </si>
   <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>ad iusto omnis odit dolor voluptatibus</t>
+    <t>89</t>
+  </si>
+  <si>
+    <t>sint soluta et vel magnam aut ut sed qui</t>
   </si>
   <si>
     <t>minus omnis soluta quia
@@ -1106,10 +1100,10 @@
 eos soluta similique molestias praesentium blanditiis</t>
   </si>
   <si>
-    <t>91</t>
-  </si>
-  <si>
-    <t>aut amet sed</t>
+    <t>90</t>
+  </si>
+  <si>
+    <t>ad iusto omnis odit dolor voluptatibus</t>
   </si>
   <si>
     <t>libero voluptate eveniet aperiam sed
@@ -1118,10 +1112,10 @@
 expedita consequatur consequatur dolores quia eos et placeat</t>
   </si>
   <si>
-    <t>92</t>
-  </si>
-  <si>
-    <t>ratione ex tenetur perferendis</t>
+    <t>91</t>
+  </si>
+  <si>
+    <t>aut amet sed</t>
   </si>
   <si>
     <t>aut et excepturi dicta laudantium sint rerum nihil
@@ -1130,10 +1124,10 @@
 commodi voluptate qui</t>
   </si>
   <si>
-    <t>93</t>
-  </si>
-  <si>
-    <t>beatae soluta recusandae</t>
+    <t>92</t>
+  </si>
+  <si>
+    <t>ratione ex tenetur perferendis</t>
   </si>
   <si>
     <t>dolorem quibusdam ducimus consequuntur dicta aut quo laboriosam
@@ -1142,10 +1136,10 @@
 sit error sed sunt eveniet provident qui nulla</t>
   </si>
   <si>
-    <t>94</t>
-  </si>
-  <si>
-    <t>qui qui voluptates illo iste minima</t>
+    <t>93</t>
+  </si>
+  <si>
+    <t>beatae soluta recusandae</t>
   </si>
   <si>
     <t>aspernatur expedita soluta quo ab ut similique
@@ -1154,10 +1148,10 @@
 omnis facilis nam ipsum natus sint similique omnis</t>
   </si>
   <si>
-    <t>95</t>
-  </si>
-  <si>
-    <t>id minus libero illum nam ad officiis</t>
+    <t>94</t>
+  </si>
+  <si>
+    <t>qui qui voluptates illo iste minima</t>
   </si>
   <si>
     <t>earum voluptatem facere provident blanditiis velit laboriosam
@@ -1166,10 +1160,10 @@
 corporis cupiditate eaque assumenda ad nesciunt</t>
   </si>
   <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>quaerat velit veniam amet cupiditate aut numquam ut sequi</t>
+    <t>95</t>
+  </si>
+  <si>
+    <t>id minus libero illum nam ad officiis</t>
   </si>
   <si>
     <t>in non odio excepturi sint eum
@@ -1178,10 +1172,10 @@
 veniam non exercitationem delectus aut</t>
   </si>
   <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>quas fugiat ut perspiciatis vero provident</t>
+    <t>96</t>
+  </si>
+  <si>
+    <t>quaerat velit veniam amet cupiditate aut numquam ut sequi</t>
   </si>
   <si>
     <t>eum non blanditiis soluta porro quibusdam voluptas
@@ -1190,10 +1184,10 @@
 perspiciatis est et voluptatem dignissimos dolor itaque sit nam</t>
   </si>
   <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>laboriosam dolor voluptates</t>
+    <t>97</t>
+  </si>
+  <si>
+    <t>quas fugiat ut perspiciatis vero provident</t>
   </si>
   <si>
     <t>doloremque ex facilis sit sint culpa
@@ -1202,10 +1196,10 @@
 veritatis est dolores</t>
   </si>
   <si>
-    <t>99</t>
-  </si>
-  <si>
-    <t>temporibus sit alias delectus eligendi possimus magni</t>
+    <t>98</t>
+  </si>
+  <si>
+    <t>laboriosam dolor voluptates</t>
   </si>
   <si>
     <t>quo deleniti praesentium dicta non quod
@@ -1214,16 +1208,22 @@
 itaque dolorem quia</t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>at nam consequatur ea labore ea harum</t>
+    <t>99</t>
+  </si>
+  <si>
+    <t>temporibus sit alias delectus eligendi possimus magni</t>
   </si>
   <si>
     <t>cupiditate quo est a modi nesciunt soluta
 ipsa voluptas error itaque dicta in
 autem qui minus magnam et distinctio eum
 accusamus ratione error aut</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>at nam consequatur ea labore ea harum</t>
   </si>
 </sst>
 </file>
@@ -1293,1399 +1293,1399 @@
         <v>4</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="0">
         <v>5</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>36</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>42</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>45</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>48</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>51</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>54</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>57</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>60</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>63</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>66</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>69</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>72</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>75</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>78</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s" s="0">
-        <v>81</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>84</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>87</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>90</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D31" t="s" s="0">
-        <v>93</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D32" t="s" s="0">
-        <v>96</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D33" t="s" s="0">
-        <v>99</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>102</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D35" t="s" s="0">
-        <v>105</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D36" t="s" s="0">
-        <v>108</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D37" t="s" s="0">
-        <v>111</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>114</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s" s="0">
-        <v>117</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D40" t="s" s="0">
-        <v>120</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D41" t="s" s="0">
-        <v>123</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>16</v>
+        <v>124</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>126</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>16</v>
+        <v>127</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D43" t="s" s="0">
-        <v>129</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D44" t="s" s="0">
-        <v>132</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>16</v>
+        <v>133</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D45" t="s" s="0">
-        <v>135</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>16</v>
+        <v>136</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>138</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>16</v>
+        <v>139</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D47" t="s" s="0">
-        <v>141</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D48" t="s" s="0">
-        <v>144</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>16</v>
+        <v>145</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D49" t="s" s="0">
-        <v>147</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>16</v>
+        <v>148</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>150</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D51" t="s" s="0">
-        <v>153</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D52" t="s" s="0">
-        <v>156</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D53" t="s" s="0">
-        <v>159</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>19</v>
+        <v>160</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>162</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>19</v>
+        <v>163</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D55" t="s" s="0">
-        <v>165</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>19</v>
+        <v>166</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D56" t="s" s="0">
-        <v>168</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>19</v>
+        <v>169</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D57" t="s" s="0">
-        <v>171</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>19</v>
+        <v>172</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>174</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D59" t="s" s="0">
-        <v>177</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D60" t="s" s="0">
-        <v>180</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>19</v>
+        <v>181</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D61" t="s" s="0">
-        <v>183</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>22</v>
+        <v>184</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C62" t="s" s="0">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>186</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>22</v>
+        <v>187</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C63" t="s" s="0">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D63" t="s" s="0">
-        <v>189</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>22</v>
+        <v>190</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D64" t="s" s="0">
-        <v>192</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>22</v>
+        <v>193</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D65" t="s" s="0">
-        <v>195</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>22</v>
+        <v>196</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D66" t="s" s="0">
-        <v>198</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>22</v>
+        <v>199</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D67" t="s" s="0">
-        <v>201</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>22</v>
+        <v>202</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D68" t="s" s="0">
-        <v>204</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>22</v>
+        <v>205</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D69" t="s" s="0">
-        <v>207</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>22</v>
+        <v>208</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C70" t="s" s="0">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D70" t="s" s="0">
-        <v>210</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>22</v>
+        <v>211</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C71" t="s" s="0">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D71" t="s" s="0">
-        <v>213</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>25</v>
+        <v>214</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D72" t="s" s="0">
-        <v>216</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>25</v>
+        <v>217</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C73" t="s" s="0">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D73" t="s" s="0">
-        <v>219</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>25</v>
+        <v>220</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C74" t="s" s="0">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D74" t="s" s="0">
-        <v>222</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>25</v>
+        <v>223</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C75" t="s" s="0">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D75" t="s" s="0">
-        <v>225</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>25</v>
+        <v>226</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C76" t="s" s="0">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D76" t="s" s="0">
-        <v>228</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>25</v>
+        <v>229</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C77" t="s" s="0">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D77" t="s" s="0">
-        <v>231</v>
+        <v>26</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s" s="0">
-        <v>25</v>
+        <v>232</v>
       </c>
       <c r="B78" t="s" s="0">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C78" t="s" s="0">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D78" t="s" s="0">
-        <v>234</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s" s="0">
-        <v>25</v>
+        <v>235</v>
       </c>
       <c r="B79" t="s" s="0">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C79" t="s" s="0">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D79" t="s" s="0">
-        <v>237</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s" s="0">
-        <v>25</v>
+        <v>238</v>
       </c>
       <c r="B80" t="s" s="0">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C80" t="s" s="0">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D80" t="s" s="0">
-        <v>240</v>
+        <v>26</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s" s="0">
-        <v>25</v>
+        <v>241</v>
       </c>
       <c r="B81" t="s" s="0">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C81" t="s" s="0">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D81" t="s" s="0">
-        <v>243</v>
+        <v>26</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s" s="0">
-        <v>28</v>
+        <v>244</v>
       </c>
       <c r="B82" t="s" s="0">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C82" t="s" s="0">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D82" t="s" s="0">
-        <v>246</v>
+        <v>29</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s" s="0">
-        <v>28</v>
+        <v>247</v>
       </c>
       <c r="B83" t="s" s="0">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C83" t="s" s="0">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D83" t="s" s="0">
-        <v>249</v>
+        <v>29</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s" s="0">
-        <v>28</v>
+        <v>250</v>
       </c>
       <c r="B84" t="s" s="0">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C84" t="s" s="0">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D84" t="s" s="0">
-        <v>252</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s" s="0">
-        <v>28</v>
+        <v>253</v>
       </c>
       <c r="B85" t="s" s="0">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C85" t="s" s="0">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D85" t="s" s="0">
-        <v>255</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s" s="0">
-        <v>28</v>
+        <v>256</v>
       </c>
       <c r="B86" t="s" s="0">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C86" t="s" s="0">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D86" t="s" s="0">
-        <v>258</v>
+        <v>29</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s" s="0">
-        <v>28</v>
+        <v>259</v>
       </c>
       <c r="B87" t="s" s="0">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C87" t="s" s="0">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D87" t="s" s="0">
-        <v>261</v>
+        <v>29</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s" s="0">
-        <v>28</v>
+        <v>262</v>
       </c>
       <c r="B88" t="s" s="0">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C88" t="s" s="0">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D88" t="s" s="0">
-        <v>264</v>
+        <v>29</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s" s="0">
-        <v>28</v>
+        <v>265</v>
       </c>
       <c r="B89" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C89" t="s" s="0">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D89" t="s" s="0">
-        <v>267</v>
+        <v>29</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s" s="0">
-        <v>28</v>
+        <v>268</v>
       </c>
       <c r="B90" t="s" s="0">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C90" t="s" s="0">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D90" t="s" s="0">
-        <v>270</v>
+        <v>29</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s" s="0">
-        <v>28</v>
+        <v>271</v>
       </c>
       <c r="B91" t="s" s="0">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C91" t="s" s="0">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D91" t="s" s="0">
-        <v>273</v>
+        <v>29</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s" s="0">
-        <v>31</v>
+        <v>274</v>
       </c>
       <c r="B92" t="s" s="0">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C92" t="s" s="0">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D92" t="s" s="0">
-        <v>276</v>
+        <v>32</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s" s="0">
-        <v>31</v>
+        <v>277</v>
       </c>
       <c r="B93" t="s" s="0">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C93" t="s" s="0">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D93" t="s" s="0">
-        <v>279</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s" s="0">
-        <v>31</v>
+        <v>280</v>
       </c>
       <c r="B94" t="s" s="0">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C94" t="s" s="0">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D94" t="s" s="0">
-        <v>282</v>
+        <v>32</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s" s="0">
-        <v>31</v>
+        <v>283</v>
       </c>
       <c r="B95" t="s" s="0">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C95" t="s" s="0">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D95" t="s" s="0">
-        <v>285</v>
+        <v>32</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s" s="0">
-        <v>31</v>
+        <v>286</v>
       </c>
       <c r="B96" t="s" s="0">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C96" t="s" s="0">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D96" t="s" s="0">
-        <v>288</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s" s="0">
-        <v>31</v>
+        <v>289</v>
       </c>
       <c r="B97" t="s" s="0">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C97" t="s" s="0">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D97" t="s" s="0">
-        <v>291</v>
+        <v>32</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s" s="0">
-        <v>31</v>
+        <v>292</v>
       </c>
       <c r="B98" t="s" s="0">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C98" t="s" s="0">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D98" t="s" s="0">
-        <v>294</v>
+        <v>32</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s" s="0">
-        <v>31</v>
+        <v>295</v>
       </c>
       <c r="B99" t="s" s="0">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C99" t="s" s="0">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D99" t="s" s="0">
-        <v>297</v>
+        <v>32</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s" s="0">
-        <v>31</v>
+        <v>298</v>
       </c>
       <c r="B100" t="s" s="0">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C100" t="s" s="0">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D100" t="s" s="0">
-        <v>300</v>
+        <v>32</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s" s="0">
-        <v>31</v>
+        <v>301</v>
       </c>
       <c r="B101" t="s" s="0">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C101" t="s" s="0">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D101" t="s" s="0">
-        <v>303</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>